<commit_message>
Created subcategory fragment, developed layouts further
</commit_message>
<xml_diff>
--- a/Extra/CouplesConnect.xlsx
+++ b/Extra/CouplesConnect.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="22995" windowHeight="12090" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="20370" windowHeight="8205" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Questions" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
   <si>
     <t>Category</t>
   </si>
@@ -117,9 +117,6 @@
     <t>Friends, Family, Partners, Strangers, Humankind, Parenting, Kids, Coworkers, Nature, Pets</t>
   </si>
   <si>
-    <t>Money, School, Work, Hygiene, Cleanliness, Organization, Fitness, Health, Diet, Hobbies, Music, Entertainment, Art, Dress, Sports, Technology,</t>
-  </si>
-  <si>
     <t xml:space="preserve">Rights, Laws, Leaders, Militarty, Security, Aid, Foreign Policy, Economy, Budgets, Prisons, Courts, Justice, Law Enforcment, </t>
   </si>
   <si>
@@ -139,6 +136,15 @@
   </si>
   <si>
     <t>Childhood</t>
+  </si>
+  <si>
+    <t>Affirmations</t>
+  </si>
+  <si>
+    <t>Needs</t>
+  </si>
+  <si>
+    <t>Money, School, Work, Hygiene, Cleanliness, Organization, Fitness, Health, Diet, Hobbies, Music, Entertainment, Art, Dress, Sports, Technology, Values</t>
   </si>
 </sst>
 </file>
@@ -552,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -584,7 +590,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -625,7 +631,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -633,7 +639,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -647,7 +653,7 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="4"/>
     </row>
@@ -672,7 +678,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D17" s="4"/>
     </row>
@@ -688,7 +694,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -703,7 +709,17 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -712,7 +728,7 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D28" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added temp fragment skeleton for adding questions; added methods for action bar
</commit_message>
<xml_diff>
--- a/Extra/CouplesConnect.xlsx
+++ b/Extra/CouplesConnect.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Category</t>
   </si>
@@ -97,9 +97,6 @@
   </si>
   <si>
     <t>God, Sin, Eternality, Life, Death, Morality, Humanity, Self, Values, Philosophy</t>
-  </si>
-  <si>
-    <t>Situations</t>
   </si>
   <si>
     <t>Nature, Environment, Earth, Culture, Society, Travel, Race, Language</t>
@@ -558,7 +555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
@@ -590,7 +587,7 @@
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D2" s="4"/>
     </row>
@@ -599,7 +596,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -615,7 +612,7 @@
         <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -631,7 +628,7 @@
         <v>22</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -639,12 +636,7 @@
         <v>24</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -653,23 +645,23 @@
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -678,7 +670,7 @@
       </c>
       <c r="B17" s="3"/>
       <c r="C17" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="4"/>
     </row>
@@ -694,7 +686,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -709,17 +701,17 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -728,7 +720,7 @@
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D28" s="4"/>
     </row>

</xml_diff>